<commit_message>
fix: Grafico de Gantt e Métricas e Estimativas
</commit_message>
<xml_diff>
--- a/Gerente/Gráfico de Gantt.xlsx
+++ b/Gerente/Gráfico de Gantt.xlsx
@@ -986,6 +986,7 @@
   <sheetPr>
     <tabColor rgb="FF3D85C6"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -994,7 +995,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="4.25"/>
     <col customWidth="1" min="2" max="2" width="11.13"/>
-    <col customWidth="1" min="3" max="3" width="36.0"/>
+    <col customWidth="1" min="3" max="3" width="34.75"/>
     <col customWidth="1" min="4" max="4" width="16.25"/>
     <col customWidth="1" min="5" max="6" width="10.5"/>
     <col customWidth="1" min="7" max="7" width="8.63"/>
@@ -2000,7 +2001,7 @@
         <v>4</v>
       </c>
       <c r="H13" s="74">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="I13" s="75"/>
       <c r="J13" s="76"/>
@@ -2086,7 +2087,7 @@
         <v>4</v>
       </c>
       <c r="H14" s="74">
-        <v>0.33</v>
+        <v>0.1</v>
       </c>
       <c r="I14" s="75"/>
       <c r="J14" s="76"/>
@@ -4495,13 +4496,30 @@
   </sheetData>
   <mergeCells count="33">
     <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I2:N2"/>
     <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="P5:AA5"/>
     <mergeCell ref="I4:O4"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
     <mergeCell ref="E8:E10"/>
     <mergeCell ref="F8:F10"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="S9:W9"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
+    <mergeCell ref="BB9:BF9"/>
+    <mergeCell ref="BG9:BK9"/>
     <mergeCell ref="G8:G10"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="I8:W8"/>
@@ -4509,24 +4527,7 @@
     <mergeCell ref="AM8:BA8"/>
     <mergeCell ref="BB8:BP8"/>
     <mergeCell ref="I9:M9"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="P5:AA5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="BB9:BF9"/>
-    <mergeCell ref="BG9:BK9"/>
     <mergeCell ref="BL9:BP9"/>
-    <mergeCell ref="S9:W9"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
   </mergeCells>
   <conditionalFormatting sqref="H12:H18 H20:H41">
     <cfRule type="colorScale" priority="1">
@@ -4548,6 +4549,9 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>